<commit_message>
checking it item is OOS or NA (funciona)
</commit_message>
<xml_diff>
--- a/Week-2/RoSA/ExcelFiles/VendorItems.xlsx
+++ b/Week-2/RoSA/ExcelFiles/VendorItems.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Dan-Vega-Code\Week-2\RoSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Dan-Vega-Code\Week-2\RoSA\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BA07AC-6D09-4A31-80A1-F6674451C3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42F4CB1-D79D-4143-A9D1-CD8AFD2A7FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="8655" windowWidth="12420" windowHeight="6840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WalMart" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Vendor</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>QtyAvailable</t>
-  </si>
-  <si>
     <t>CVS</t>
   </si>
   <si>
@@ -78,14 +75,28 @@
   </si>
   <si>
     <t>Pain Reliever</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -113,8 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +408,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,21 +422,22 @@
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -432,18 +445,18 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>88</v>
@@ -452,15 +465,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>109</v>
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -475,6 +488,7 @@
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -482,7 +496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCE7850-F426-48A9-A048-A61D12A47C29}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -493,25 +509,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -522,10 +538,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>88</v>
@@ -536,10 +552,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>109</v>
@@ -550,6 +566,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -558,7 +575,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,29 +583,29 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2">
         <v>13</v>
@@ -599,10 +616,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>25</v>
@@ -613,10 +630,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>16</v>

</xml_diff>

<commit_message>
Noy hay o no existe
</commit_message>
<xml_diff>
--- a/Week-2/RoSA/ExcelFiles/VendorItems.xlsx
+++ b/Week-2/RoSA/ExcelFiles/VendorItems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Dan-Vega-Code\Week-2\RoSA\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42F4CB1-D79D-4143-A9D1-CD8AFD2A7FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB368050-F891-48B4-A206-5866EE1F1508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11370" yWindow="5265" windowWidth="15090" windowHeight="7980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WalMart" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>Vendor</t>
   </si>
@@ -410,7 +410,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -497,7 +497,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>12</v>
@@ -557,8 +557,8 @@
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4">
-        <v>109</v>
+      <c r="C4" t="s">
+        <v>16</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1BE07A-019F-47AC-9A68-990ADD02B1F7}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,8 +607,8 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>13</v>
+      <c r="C2" t="s">
+        <v>16</v>
       </c>
       <c r="D2">
         <v>27</v>
@@ -636,7 +636,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>23</v>

</xml_diff>